<commit_message>
Updated Sprint Backlog and Burndown Chart
</commit_message>
<xml_diff>
--- a/Phase 1/Sprint1/Burndown Chart.xlsx
+++ b/Phase 1/Sprint1/Burndown Chart.xlsx
@@ -269,11 +269,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="594499491"/>
-        <c:axId val="1606407964"/>
+        <c:axId val="1793078072"/>
+        <c:axId val="996771503"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="594499491"/>
+        <c:axId val="1793078072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -325,10 +325,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1606407964"/>
+        <c:crossAx val="996771503"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1606407964"/>
+        <c:axId val="996771503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,7 +392,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594499491"/>
+        <c:crossAx val="1793078072"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -815,7 +815,7 @@
         <v>0.0</v>
       </c>
       <c r="H6" s="5">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I6" s="5"/>
     </row>
@@ -975,11 +975,11 @@
       </c>
       <c r="H17" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I17" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated Scrum files and also patterns and code smells
</commit_message>
<xml_diff>
--- a/Phase 1/Sprint1/Burndown Chart.xlsx
+++ b/Phase 1/Sprint1/Burndown Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>BackLog ID</t>
   </si>
@@ -32,12 +32,50 @@
   <si>
     <t>2 - For Docs 2 - For Reviews</t>
   </si>
+  <si>
+    <t>BackLog IDs</t>
+  </si>
+  <si>
+    <t>Identify 3 patterns and
+ three code smells (id 1)</t>
+  </si>
+  <si>
+    <t>Rafael Martins</t>
+  </si>
+  <si>
+    <t>Identify 3 patterns and
+ three code smells (id 2)</t>
+  </si>
+  <si>
+    <t>Rafael Pereira</t>
+  </si>
+  <si>
+    <t>Identify 3 patterns and
+ three code smells (id 3)</t>
+  </si>
+  <si>
+    <t>Guilherme</t>
+  </si>
+  <si>
+    <t>Identify 3 patterns and
+ three code smells (id 4)</t>
+  </si>
+  <si>
+    <t>Pedro Fernandes</t>
+  </si>
+  <si>
+    <t>Identify 3 patterns and
+ three code smells (id 5)</t>
+  </si>
+  <si>
+    <t>Pedro Lopes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -53,8 +91,9 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,8 +118,50 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6FA8DC"/>
+        <bgColor rgb="FF6FA8DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC9696"/>
+        <bgColor rgb="FFFC9696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD6EE"/>
+        <bgColor rgb="FFBDD6EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5E0B3"/>
+        <bgColor rgb="FFC5E0B3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7CAAC"/>
+        <bgColor rgb="FFF7CAAC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE598"/>
+        <bgColor rgb="FFFFE598"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border/>
     <border>
       <left style="medium">
@@ -115,6 +196,33 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -123,10 +231,14 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -135,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -150,22 +262,61 @@
     <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="2" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="6" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="6" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="5" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="7" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -231,7 +382,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$I$17</c:f>
+              <c:f>Sheet1!$B$8:$I$8</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -260,17 +411,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$I$18</c:f>
+              <c:f>Sheet1!$B$9:$I$9</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="17638216"/>
-        <c:axId val="1920773233"/>
+        <c:axId val="1519336200"/>
+        <c:axId val="236351578"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17638216"/>
+        <c:axId val="1519336200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,10 +473,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1920773233"/>
+        <c:crossAx val="236351578"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1920773233"/>
+        <c:axId val="236351578"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -389,7 +540,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17638216"/>
+        <c:crossAx val="1519336200"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -419,10 +570,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4371975" cy="2714625"/>
     <xdr:graphicFrame>
@@ -650,9 +801,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.71"/>
-    <col customWidth="1" min="2" max="2" width="11.86"/>
-    <col customWidth="1" min="3" max="3" width="16.14"/>
-    <col customWidth="1" min="4" max="9" width="12.57"/>
+    <col customWidth="1" min="2" max="2" width="18.57"/>
+    <col customWidth="1" min="3" max="9" width="17.0"/>
     <col customWidth="1" min="10" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -733,7 +883,9 @@
       <c r="H3" s="4">
         <v>0.0</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="4">
@@ -818,7 +970,9 @@
       <c r="H6" s="4">
         <v>2.0</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="4">
@@ -845,187 +999,197 @@
       <c r="H7" s="4">
         <v>0.0</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <f>SUM(B3:B7)</f>
+        <v>20</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" ref="C8:I8" si="1">B8-SUM(C3:C7)</f>
+        <v>20</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="A9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="9">
+        <f>SUM(B3:B7)</f>
+        <v>20</v>
+      </c>
+      <c r="C9" s="10">
+        <f>B9-(B9/7*C2)</f>
+        <v>17.14285714</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" ref="D9:I9" si="2">$B9-($B9/7*D2)</f>
+        <v>14.28571429</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="2"/>
+        <v>11.42857143</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="2"/>
+        <v>8.571428571</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" si="2"/>
+        <v>5.714285714</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="2"/>
+        <v>2.857142857</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="A11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+    <row r="12" ht="21.75" customHeight="1">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+    <row r="13" ht="1.5" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+    <row r="14" ht="20.25" customHeight="1">
+      <c r="A14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+    <row r="15" ht="30.75" customHeight="1">
+      <c r="A15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="D15" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+    <row r="16" ht="30.75" customHeight="1">
+      <c r="A16" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="D16" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="9">
-        <f>SUM(B3:B16)</f>
-        <v>20</v>
-      </c>
-      <c r="C17" s="9">
-        <f t="shared" ref="C17:I17" si="1">B17-SUM(C3:C16)</f>
-        <v>20</v>
-      </c>
-      <c r="D17" s="9">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="E17" s="9">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="F17" s="9">
-        <f t="shared" si="1"/>
+    <row r="17" ht="30.75" customHeight="1">
+      <c r="A17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="D17" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" ht="30.75" customHeight="1">
+      <c r="A18" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="D18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="9">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="H17" s="9">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="I17" s="9">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="9">
-        <f>SUM(B3:B16)</f>
-        <v>20</v>
-      </c>
-      <c r="C18" s="12">
-        <f>B18-(B18/7*C2)</f>
-        <v>17.14285714</v>
-      </c>
-      <c r="D18" s="12">
-        <f t="shared" ref="D18:I18" si="2">$B18-($B18/7*D2)</f>
-        <v>14.28571429</v>
-      </c>
-      <c r="E18" s="12">
-        <f t="shared" si="2"/>
-        <v>11.42857143</v>
-      </c>
-      <c r="F18" s="12">
-        <f t="shared" si="2"/>
-        <v>8.571428571</v>
-      </c>
-      <c r="G18" s="12">
-        <f t="shared" si="2"/>
-        <v>5.714285714</v>
-      </c>
-      <c r="H18" s="12">
-        <f t="shared" si="2"/>
-        <v>2.857142857</v>
-      </c>
-      <c r="I18" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+    <row r="19" ht="30.75" customHeight="1">
+      <c r="A19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="D19" s="28" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1"/>
     <row r="22" ht="14.25" customHeight="1"/>
     <row r="23" ht="14.25" customHeight="1"/>
@@ -2007,6 +2171,14 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A14:B14"/>
+  </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>

</xml_diff>